<commit_message>
More finetunes on Emissions
</commit_message>
<xml_diff>
--- a/suppxls/Scen_CombustionEmissions.xlsx
+++ b/suppxls/Scen_CombustionEmissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84786141-F5AC-4A02-9283-724B942F9370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA5B4A2-10A5-4895-AF50-A2A052A36F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2190" yWindow="2460" windowWidth="26610" windowHeight="13740" xr2:uid="{5C169CAC-8982-47AA-A2BD-20E5E721E68B}"/>
   </bookViews>
@@ -292,10 +292,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -377,7 +376,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -387,7 +386,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading 2 2 2" xfId="1" xr:uid="{39415C90-2BAA-44BE-A516-ED7D1B21DDFA}"/>
@@ -1749,7 +1747,7 @@
       <selection activeCell="B17" sqref="B17:I35"/>
       <selection pane="topRight" activeCell="B17" sqref="B17:I35"/>
       <selection pane="bottomLeft" activeCell="B17" sqref="B17:I35"/>
-      <selection pane="bottomRight" activeCell="P17" sqref="P17:P18"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,8 +2170,8 @@
         <v>CO2C</v>
       </c>
       <c r="P17">
-        <f>C6</f>
-        <v>96.25</v>
+        <f>J6</f>
+        <v>72.900000000000006</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -2210,9 +2208,9 @@
         <f t="shared" ref="O18:O23" si="0">B7</f>
         <v>CH4C</v>
       </c>
-      <c r="P18" s="7">
-        <f t="shared" ref="P18:P23" si="1">C7</f>
-        <v>1E-3</v>
+      <c r="P18">
+        <f t="shared" ref="P18:P24" si="1">J7</f>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -2251,7 +2249,7 @@
       </c>
       <c r="P19">
         <f t="shared" si="1"/>
-        <v>1.4E-3</v>
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -2290,7 +2288,7 @@
       </c>
       <c r="P20">
         <f t="shared" si="1"/>
-        <v>0.62619999999999998</v>
+        <v>4.5900000000000003E-2</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -2329,7 +2327,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -2368,7 +2366,7 @@
       </c>
       <c r="P22">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
@@ -2445,8 +2443,8 @@
         <v>PM10S</v>
       </c>
       <c r="P24">
-        <f>C13</f>
-        <v>4.5769644752755773E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>